<commit_message>
update new test cases
</commit_message>
<xml_diff>
--- a/updated_Vung-Khuvuc.xlsx
+++ b/updated_Vung-Khuvuc.xlsx
@@ -1351,7 +1351,11 @@
           <t>Quận Tân Bình, TP.HCM</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr"/>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C73" t="inlineStr"/>
     </row>
     <row r="74">
@@ -1360,7 +1364,11 @@
           <t>Quận Tân Bình TPHCM</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr"/>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C74" t="inlineStr"/>
     </row>
     <row r="75">
@@ -1369,7 +1377,11 @@
           <t>Quận 7, TP HCM</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr"/>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C75" t="inlineStr"/>
     </row>
     <row r="76">
@@ -1378,7 +1390,11 @@
           <t>Quận 4 TPHCM</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr"/>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C76" t="inlineStr"/>
     </row>
     <row r="77">
@@ -1387,7 +1403,11 @@
           <t>Tp. HCM</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr"/>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C77" t="inlineStr"/>
     </row>
     <row r="78">
@@ -1409,7 +1429,11 @@
           <t>Q. Bình Thạnh, TP. HCM</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr"/>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C79" t="inlineStr"/>
     </row>
     <row r="80">
@@ -1418,7 +1442,11 @@
           <t>Quận 7, TP. HCM</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr"/>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C80" t="inlineStr"/>
     </row>
     <row r="81">
@@ -1488,7 +1516,11 @@
           <t>Nhà Bè, TpHCM</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr"/>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C86" t="inlineStr"/>
     </row>
     <row r="87">
@@ -1619,7 +1651,11 @@
           <t>tp. Thủ Đức tp. HCM</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr"/>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C97" t="inlineStr"/>
     </row>
     <row r="98">
@@ -1747,7 +1783,11 @@
           <t>Tp HCM</t>
         </is>
       </c>
-      <c r="B109" t="inlineStr"/>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C109" t="inlineStr"/>
     </row>
     <row r="110">
@@ -1769,7 +1809,11 @@
           <t>TP. HCM</t>
         </is>
       </c>
-      <c r="B111" t="inlineStr"/>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C111" t="inlineStr"/>
     </row>
     <row r="112">
@@ -1891,7 +1935,11 @@
           <t>Tp hcm</t>
         </is>
       </c>
-      <c r="B121" t="inlineStr"/>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C121" t="inlineStr"/>
     </row>
     <row r="122">
@@ -2158,7 +2206,11 @@
           <t>TpHCM</t>
         </is>
       </c>
-      <c r="B144" t="inlineStr"/>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C144" t="inlineStr"/>
     </row>
     <row r="145">
@@ -2310,7 +2362,11 @@
           <t>TP HCM</t>
         </is>
       </c>
-      <c r="B156" t="inlineStr"/>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C156" t="inlineStr"/>
     </row>
     <row r="157">
@@ -2341,7 +2397,11 @@
           <t>quận 12, Tp.HCM</t>
         </is>
       </c>
-      <c r="B159" t="inlineStr"/>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C159" t="inlineStr"/>
     </row>
     <row r="160">
@@ -2350,7 +2410,11 @@
           <t>Tphcm</t>
         </is>
       </c>
-      <c r="B160" t="inlineStr"/>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C160" t="inlineStr"/>
     </row>
     <row r="161">
@@ -2359,7 +2423,11 @@
           <t>Q10, TPHCM</t>
         </is>
       </c>
-      <c r="B161" t="inlineStr"/>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C161" t="inlineStr"/>
     </row>
     <row r="162">
@@ -2586,7 +2654,11 @@
           <t>Quận 7, TP HCM</t>
         </is>
       </c>
-      <c r="B180" t="inlineStr"/>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C180" t="inlineStr"/>
     </row>
     <row r="181">
@@ -2617,7 +2689,11 @@
           <t>TP HCM</t>
         </is>
       </c>
-      <c r="B183" t="inlineStr"/>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C183" t="inlineStr"/>
     </row>
     <row r="184">
@@ -2626,7 +2702,11 @@
           <t>Quận 8, HCM</t>
         </is>
       </c>
-      <c r="B184" t="inlineStr"/>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C184" t="inlineStr"/>
     </row>
     <row r="185">
@@ -2797,7 +2877,11 @@
           <t>Xuyên Mộc, Brvt</t>
         </is>
       </c>
-      <c r="B199" t="inlineStr"/>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C199" t="inlineStr"/>
     </row>
     <row r="200">
@@ -2893,7 +2977,11 @@
           <t>huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B207" t="inlineStr"/>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C207" t="inlineStr"/>
     </row>
     <row r="208">
@@ -2911,7 +2999,11 @@
           <t>Huyện Long Điền tỉnh brvt</t>
         </is>
       </c>
-      <c r="B209" t="inlineStr"/>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C209" t="inlineStr"/>
     </row>
     <row r="210">
@@ -2933,7 +3025,11 @@
           <t>huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B211" t="inlineStr"/>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C211" t="inlineStr"/>
     </row>
     <row r="212">
@@ -2942,7 +3038,11 @@
           <t>LONG DIEN - BRVT</t>
         </is>
       </c>
-      <c r="B212" t="inlineStr"/>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C212" t="inlineStr"/>
     </row>
     <row r="213">
@@ -2951,7 +3051,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B213" t="inlineStr"/>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C213" t="inlineStr"/>
     </row>
     <row r="214">
@@ -3052,7 +3156,11 @@
           <t>Xuyên Mộc BRVT</t>
         </is>
       </c>
-      <c r="B222" t="inlineStr"/>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C222" t="inlineStr"/>
     </row>
     <row r="223">
@@ -3171,7 +3279,11 @@
           <t>Huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B233" t="inlineStr"/>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C233" t="inlineStr"/>
     </row>
     <row r="234">
@@ -3320,7 +3432,11 @@
           <t>Tỉnh brvt</t>
         </is>
       </c>
-      <c r="B246" t="inlineStr"/>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C246" t="inlineStr"/>
     </row>
     <row r="247">
@@ -3329,7 +3445,11 @@
           <t>Long Điền,BRVT</t>
         </is>
       </c>
-      <c r="B247" t="inlineStr"/>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C247" t="inlineStr"/>
     </row>
     <row r="248">
@@ -3434,7 +3554,11 @@
           <t>Long Điền- BRVT</t>
         </is>
       </c>
-      <c r="B256" t="inlineStr"/>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C256" t="inlineStr"/>
     </row>
     <row r="257">
@@ -3587,7 +3711,11 @@
           <t>Huyện Xuyên Mộc, Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B269" t="inlineStr"/>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C269" t="inlineStr"/>
     </row>
     <row r="270">
@@ -3596,7 +3724,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B270" t="inlineStr"/>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C270" t="inlineStr"/>
     </row>
     <row r="271">
@@ -3710,7 +3842,11 @@
           <t>Huyện Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B280" t="inlineStr"/>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C280" t="inlineStr"/>
     </row>
     <row r="281">
@@ -3876,7 +4012,11 @@
           <t>Huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B294" t="inlineStr"/>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C294" t="inlineStr"/>
     </row>
     <row r="295">
@@ -3911,7 +4051,11 @@
           <t>Huyện long điền tỉnh brvt</t>
         </is>
       </c>
-      <c r="B297" t="inlineStr"/>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C297" t="inlineStr"/>
     </row>
     <row r="298">
@@ -3973,7 +4117,11 @@
           <t>Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B303" t="inlineStr"/>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C303" t="inlineStr"/>
     </row>
     <row r="304">
@@ -4173,7 +4321,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B319" t="inlineStr"/>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C319" t="inlineStr"/>
     </row>
     <row r="320">
@@ -4265,7 +4417,11 @@
           <t>Long ĐIỀN BRVT</t>
         </is>
       </c>
-      <c r="B327" t="inlineStr"/>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C327" t="inlineStr"/>
     </row>
     <row r="328">
@@ -4374,7 +4530,11 @@
           <t>Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B336" t="inlineStr"/>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C336" t="inlineStr"/>
     </row>
     <row r="337">
@@ -4474,7 +4634,11 @@
           <t>Xuyên Mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B344" t="inlineStr"/>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C344" t="inlineStr"/>
     </row>
     <row r="345">
@@ -4675,7 +4839,11 @@
           <t>Xuyên Mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B361" t="inlineStr"/>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C361" t="inlineStr"/>
     </row>
     <row r="362">
@@ -4697,7 +4865,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B363" t="inlineStr"/>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C363" t="inlineStr"/>
     </row>
     <row r="364">
@@ -4706,7 +4878,11 @@
           <t>Huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B364" t="inlineStr"/>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C364" t="inlineStr"/>
     </row>
     <row r="365">
@@ -4754,7 +4930,11 @@
           <t>Huyện Châu Đức- Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B368" t="inlineStr"/>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C368" t="inlineStr"/>
     </row>
     <row r="369">
@@ -4986,7 +5166,11 @@
           <t>XUYÊN MỘC, BRVT</t>
         </is>
       </c>
-      <c r="B388" t="inlineStr"/>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C388" t="inlineStr"/>
     </row>
     <row r="389">
@@ -5109,7 +5293,11 @@
           <t>Huyện Long Điền-Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B399" t="inlineStr"/>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C399" t="inlineStr"/>
     </row>
     <row r="400">
@@ -5131,7 +5319,11 @@
           <t>Huyện Long Điền- BRVT</t>
         </is>
       </c>
-      <c r="B401" t="inlineStr"/>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C401" t="inlineStr"/>
     </row>
     <row r="402">
@@ -5197,7 +5389,11 @@
           <t>Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B407" t="inlineStr"/>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C407" t="inlineStr"/>
     </row>
     <row r="408">
@@ -5276,7 +5472,11 @@
           <t>Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B414" t="inlineStr"/>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C414" t="inlineStr"/>
     </row>
     <row r="415">
@@ -5433,7 +5633,11 @@
           <t>Huyện Xuyên Mộc. BRVT</t>
         </is>
       </c>
-      <c r="B427" t="inlineStr"/>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C427" t="inlineStr"/>
     </row>
     <row r="428">
@@ -5665,7 +5869,11 @@
           <t>Hcm</t>
         </is>
       </c>
-      <c r="B447" t="inlineStr"/>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C447" t="inlineStr"/>
     </row>
     <row r="448">
@@ -5731,7 +5939,11 @@
           <t>Quận 10, TPHCM</t>
         </is>
       </c>
-      <c r="B453" t="inlineStr"/>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C453" t="inlineStr"/>
     </row>
     <row r="454">
@@ -5845,7 +6057,11 @@
           <t>Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B463" t="inlineStr"/>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C463" t="inlineStr"/>
     </row>
     <row r="464">
@@ -5906,7 +6122,11 @@
           <t>Tp HCM</t>
         </is>
       </c>
-      <c r="B468" t="inlineStr"/>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C468" t="inlineStr"/>
     </row>
     <row r="469">
@@ -5976,7 +6196,11 @@
           <t>TP. HCM</t>
         </is>
       </c>
-      <c r="B474" t="inlineStr"/>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C474" t="inlineStr"/>
     </row>
     <row r="475">
@@ -6115,7 +6339,11 @@
           <t>Huyện Xuyên mộc, Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B485" t="inlineStr"/>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C485" t="inlineStr"/>
     </row>
     <row r="486">
@@ -6146,7 +6374,11 @@
           <t>Huyện Long Điền- BRVT</t>
         </is>
       </c>
-      <c r="B488" t="inlineStr"/>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C488" t="inlineStr"/>
     </row>
     <row r="489">
@@ -6351,7 +6583,11 @@
           <t>Huyện Long Điền, Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B505" t="inlineStr"/>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C505" t="inlineStr"/>
     </row>
     <row r="506">
@@ -6779,7 +7015,11 @@
           <t>XUYÊN MỘC, BRVT</t>
         </is>
       </c>
-      <c r="B541" t="inlineStr"/>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C541" t="inlineStr"/>
     </row>
     <row r="542">
@@ -6801,7 +7041,11 @@
           <t>Xuyên mộc_ brvt</t>
         </is>
       </c>
-      <c r="B543" t="inlineStr"/>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C543" t="inlineStr"/>
     </row>
     <row r="544">
@@ -6849,7 +7093,11 @@
           <t>Đất Đỏ, BRVT</t>
         </is>
       </c>
-      <c r="B547" t="inlineStr"/>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C547" t="inlineStr"/>
     </row>
     <row r="548">
@@ -6915,7 +7163,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B553" t="inlineStr"/>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C553" t="inlineStr"/>
     </row>
     <row r="554">
@@ -6950,7 +7202,11 @@
           <t>Xuyên mộc, brvt</t>
         </is>
       </c>
-      <c r="B556" t="inlineStr"/>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C556" t="inlineStr"/>
     </row>
     <row r="557">
@@ -7020,7 +7276,11 @@
           <t>Xuyên Mộc ,BRVT</t>
         </is>
       </c>
-      <c r="B562" t="inlineStr"/>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C562" t="inlineStr"/>
     </row>
     <row r="563">
@@ -7047,7 +7307,11 @@
           <t>TpHCM</t>
         </is>
       </c>
-      <c r="B565" t="inlineStr"/>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C565" t="inlineStr"/>
     </row>
     <row r="566">
@@ -7365,7 +7629,11 @@
           <t>TP. HCM</t>
         </is>
       </c>
-      <c r="B591" t="inlineStr"/>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C591" t="inlineStr"/>
     </row>
     <row r="592">
@@ -7374,7 +7642,11 @@
           <t>Huyện Xuyên Mộc, Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B592" t="inlineStr"/>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C592" t="inlineStr"/>
     </row>
     <row r="593">
@@ -7601,7 +7873,11 @@
           <t>TPHCM</t>
         </is>
       </c>
-      <c r="B611" t="inlineStr"/>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C611" t="inlineStr"/>
     </row>
     <row r="612">
@@ -7872,7 +8148,11 @@
           <t>Xuyên Mộc.tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B634" t="inlineStr"/>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C634" t="inlineStr"/>
     </row>
     <row r="635">
@@ -7920,7 +8200,11 @@
           <t>Huyện Xuyên Mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B638" t="inlineStr"/>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C638" t="inlineStr"/>
     </row>
     <row r="639">
@@ -8042,7 +8326,11 @@
           <t>BRVT</t>
         </is>
       </c>
-      <c r="B648" t="inlineStr"/>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C648" t="inlineStr"/>
     </row>
     <row r="649">
@@ -8090,7 +8378,11 @@
           <t>Huyện Bình Chánh, TPHCM</t>
         </is>
       </c>
-      <c r="B652" t="inlineStr"/>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C652" t="inlineStr"/>
     </row>
     <row r="653">
@@ -8504,7 +8796,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B686" t="inlineStr"/>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C686" t="inlineStr"/>
     </row>
     <row r="687">
@@ -8627,7 +8923,11 @@
           <t>Huyện xuyên mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B697" t="inlineStr"/>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C697" t="inlineStr"/>
     </row>
     <row r="698">
@@ -8784,7 +9084,11 @@
           <t>quận 6, TPHCM</t>
         </is>
       </c>
-      <c r="B710" t="inlineStr"/>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C710" t="inlineStr"/>
     </row>
     <row r="711">
@@ -8802,7 +9106,11 @@
           <t>Tx phú mỹ brvt</t>
         </is>
       </c>
-      <c r="B712" t="inlineStr"/>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C712" t="inlineStr"/>
     </row>
     <row r="713">
@@ -8876,7 +9184,11 @@
           <t>Đất Đỏ, BRVT</t>
         </is>
       </c>
-      <c r="B718" t="inlineStr"/>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C718" t="inlineStr"/>
     </row>
     <row r="719">
@@ -9059,7 +9371,11 @@
           <t>Huyện Đất Đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B733" t="inlineStr"/>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C733" t="inlineStr"/>
     </row>
     <row r="734">
@@ -9190,7 +9506,11 @@
           <t>HUYỆN LONG ĐIỀN TỈNH BRVT</t>
         </is>
       </c>
-      <c r="B744" t="inlineStr"/>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C744" t="inlineStr"/>
     </row>
     <row r="745">
@@ -9435,7 +9755,11 @@
           <t>BRVT</t>
         </is>
       </c>
-      <c r="B765" t="inlineStr"/>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C765" t="inlineStr"/>
     </row>
     <row r="766">
@@ -9540,7 +9864,11 @@
           <t>LONG ĐIỀN, BRVT</t>
         </is>
       </c>
-      <c r="B774" t="inlineStr"/>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C774" t="inlineStr"/>
     </row>
     <row r="775">
@@ -9575,7 +9903,11 @@
           <t>Châu Đức, BRVT</t>
         </is>
       </c>
-      <c r="B777" t="inlineStr"/>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C777" t="inlineStr"/>
     </row>
     <row r="778">
@@ -9584,7 +9916,11 @@
           <t>Long Điền-BRVT</t>
         </is>
       </c>
-      <c r="B778" t="inlineStr"/>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C778" t="inlineStr"/>
     </row>
     <row r="779">
@@ -9615,7 +9951,11 @@
           <t>Quận 6, TPHCM</t>
         </is>
       </c>
-      <c r="B781" t="inlineStr"/>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C781" t="inlineStr"/>
     </row>
     <row r="782">
@@ -9702,7 +10042,11 @@
           <t>Tp HCM</t>
         </is>
       </c>
-      <c r="B788" t="inlineStr"/>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C788" t="inlineStr"/>
     </row>
     <row r="789">
@@ -9924,7 +10268,11 @@
           <t>Huyện Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B806" t="inlineStr"/>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C806" t="inlineStr"/>
     </row>
     <row r="807">
@@ -9973,7 +10321,11 @@
           <t>Xuyên Mộc - BRVT</t>
         </is>
       </c>
-      <c r="B811" t="inlineStr"/>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C811" t="inlineStr"/>
     </row>
     <row r="812">
@@ -10008,7 +10360,11 @@
           <t>Xuyên Mộc - BRVT</t>
         </is>
       </c>
-      <c r="B814" t="inlineStr"/>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C814" t="inlineStr"/>
     </row>
     <row r="815">
@@ -10043,7 +10399,11 @@
           <t>Đất Đỏ BRVT</t>
         </is>
       </c>
-      <c r="B817" t="inlineStr"/>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C817" t="inlineStr"/>
     </row>
     <row r="818">
@@ -10091,7 +10451,11 @@
           <t>Đất đỏ,BRVT</t>
         </is>
       </c>
-      <c r="B821" t="inlineStr"/>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C821" t="inlineStr"/>
     </row>
     <row r="822">
@@ -10209,7 +10573,11 @@
           <t>Đất Đỏ, BRVT</t>
         </is>
       </c>
-      <c r="B831" t="inlineStr"/>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C831" t="inlineStr"/>
     </row>
     <row r="832">
@@ -10296,7 +10664,11 @@
           <t>Côn Đảo, BRVT</t>
         </is>
       </c>
-      <c r="B838" t="inlineStr"/>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C838" t="inlineStr"/>
     </row>
     <row r="839">
@@ -10314,7 +10686,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B840" t="inlineStr"/>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C840" t="inlineStr"/>
     </row>
     <row r="841">
@@ -10410,7 +10786,11 @@
           <t>BRVT</t>
         </is>
       </c>
-      <c r="B848" t="inlineStr"/>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C848" t="inlineStr"/>
     </row>
     <row r="849">
@@ -10419,7 +10799,11 @@
           <t>Quận 5, TP.HCM</t>
         </is>
       </c>
-      <c r="B849" t="inlineStr"/>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C849" t="inlineStr"/>
     </row>
     <row r="850">
@@ -10502,7 +10886,11 @@
           <t>Xuyên Mộc. BRVT.</t>
         </is>
       </c>
-      <c r="B856" t="inlineStr"/>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C856" t="inlineStr"/>
     </row>
     <row r="857">
@@ -10681,7 +11069,11 @@
           <t>Thị xã Phú Mỹ,  BRVT</t>
         </is>
       </c>
-      <c r="B871" t="inlineStr"/>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C871" t="inlineStr"/>
     </row>
     <row r="872">
@@ -10690,7 +11082,11 @@
           <t>Huyện Châu Đức, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B872" t="inlineStr"/>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C872" t="inlineStr"/>
     </row>
     <row r="873">
@@ -10721,7 +11117,11 @@
           <t>Tỉnh brvt</t>
         </is>
       </c>
-      <c r="B875" t="inlineStr"/>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C875" t="inlineStr"/>
     </row>
     <row r="876">
@@ -10791,7 +11191,11 @@
           <t>Huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B881" t="inlineStr"/>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C881" t="inlineStr"/>
     </row>
     <row r="882">
@@ -10913,7 +11317,11 @@
           <t>TpHCM</t>
         </is>
       </c>
-      <c r="B891" t="inlineStr"/>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C891" t="inlineStr"/>
     </row>
     <row r="892">
@@ -11118,7 +11526,11 @@
           <t>TX Phú Mỹ, BRVT</t>
         </is>
       </c>
-      <c r="B908" t="inlineStr"/>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C908" t="inlineStr"/>
     </row>
     <row r="909">
@@ -11149,7 +11561,11 @@
           <t>Tp. HCM</t>
         </is>
       </c>
-      <c r="B911" t="inlineStr"/>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C911" t="inlineStr"/>
     </row>
     <row r="912">
@@ -11193,7 +11609,11 @@
           <t>Huyện Xuyên Mộc- Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B915" t="inlineStr"/>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C915" t="inlineStr"/>
     </row>
     <row r="916">
@@ -11281,7 +11701,11 @@
           <t>Huyện long điền, tỉnh brvt</t>
         </is>
       </c>
-      <c r="B923" t="inlineStr"/>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C923" t="inlineStr"/>
     </row>
     <row r="924">
@@ -11360,7 +11784,11 @@
           <t>Long điền, brvt</t>
         </is>
       </c>
-      <c r="B930" t="inlineStr"/>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C930" t="inlineStr"/>
     </row>
     <row r="931">
@@ -11613,7 +12041,11 @@
           <t>LONG ĐIỀN, BRVT</t>
         </is>
       </c>
-      <c r="B951" t="inlineStr"/>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C951" t="inlineStr"/>
     </row>
     <row r="952">
@@ -11635,7 +12067,11 @@
           <t>Huyện Xuyên Mộc. Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B953" t="inlineStr"/>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C953" t="inlineStr"/>
     </row>
     <row r="954">
@@ -11657,7 +12093,11 @@
           <t>HUYỆN XUYÊN MỘC TỈNH BRVT</t>
         </is>
       </c>
-      <c r="B955" t="inlineStr"/>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C955" t="inlineStr"/>
     </row>
     <row r="956">
@@ -11697,7 +12137,11 @@
           <t>Tphcm</t>
         </is>
       </c>
-      <c r="B959" t="inlineStr"/>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C959" t="inlineStr"/>
     </row>
     <row r="960">
@@ -11706,7 +12150,11 @@
           <t>Thành phố Thủ Đức, TP HCM</t>
         </is>
       </c>
-      <c r="B960" t="inlineStr"/>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C960" t="inlineStr"/>
     </row>
     <row r="961">
@@ -11741,7 +12189,11 @@
           <t>Xuyên Mộc .Brvt</t>
         </is>
       </c>
-      <c r="B963" t="inlineStr"/>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C963" t="inlineStr"/>
     </row>
     <row r="964">
@@ -11811,7 +12263,11 @@
           <t>HUYỆN ĐẤT ĐỎ, TỈNH BRVT</t>
         </is>
       </c>
-      <c r="B969" t="inlineStr"/>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C969" t="inlineStr"/>
     </row>
     <row r="970">
@@ -11894,7 +12350,11 @@
           <t>BRVT</t>
         </is>
       </c>
-      <c r="B976" t="inlineStr"/>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C976" t="inlineStr"/>
     </row>
     <row r="977">
@@ -12038,7 +12498,11 @@
           <t>Tân Phú, TPHCM</t>
         </is>
       </c>
-      <c r="B988" t="inlineStr"/>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C988" t="inlineStr"/>
     </row>
     <row r="989">
@@ -12143,7 +12607,11 @@
           <t>Huyện Đất Đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B997" t="inlineStr"/>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C997" t="inlineStr"/>
     </row>
     <row r="998">
@@ -12453,7 +12921,11 @@
           <t>Thị xã Phú Mỹ- Brvt</t>
         </is>
       </c>
-      <c r="B1023" t="inlineStr"/>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1023" t="inlineStr"/>
     </row>
     <row r="1024">
@@ -12502,7 +12974,11 @@
           <t>Long điền- brvt</t>
         </is>
       </c>
-      <c r="B1028" t="inlineStr"/>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1028" t="inlineStr"/>
     </row>
     <row r="1029">
@@ -12607,7 +13083,11 @@
           <t>BRVT</t>
         </is>
       </c>
-      <c r="B1037" t="inlineStr"/>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1037" t="inlineStr"/>
     </row>
     <row r="1038">
@@ -12681,7 +13161,11 @@
           <t>Huyện xuyên Mộc tĩnh BRVT</t>
         </is>
       </c>
-      <c r="B1043" t="inlineStr"/>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1043" t="inlineStr"/>
     </row>
     <row r="1044">
@@ -12729,7 +13213,11 @@
           <t>TPHCM</t>
         </is>
       </c>
-      <c r="B1047" t="inlineStr"/>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1047" t="inlineStr"/>
     </row>
     <row r="1048">
@@ -12773,7 +13261,11 @@
           <t>Huyện Long Điền Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1051" t="inlineStr"/>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1051" t="inlineStr"/>
     </row>
     <row r="1052">
@@ -12843,7 +13335,11 @@
           <t>Đất Đỏ- BRVT</t>
         </is>
       </c>
-      <c r="B1057" t="inlineStr"/>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1057" t="inlineStr"/>
     </row>
     <row r="1058">
@@ -12865,7 +13361,11 @@
           <t>Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B1059" t="inlineStr"/>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1059" t="inlineStr"/>
     </row>
     <row r="1060">
@@ -13035,7 +13535,11 @@
           <t>Đất Đỏ, BRVT</t>
         </is>
       </c>
-      <c r="B1073" t="inlineStr"/>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1073" t="inlineStr"/>
     </row>
     <row r="1074">
@@ -13057,7 +13561,11 @@
           <t>Xuyên mộc- brvt</t>
         </is>
       </c>
-      <c r="B1075" t="inlineStr"/>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1075" t="inlineStr"/>
     </row>
     <row r="1076">
@@ -13066,7 +13574,11 @@
           <t>TP HCM</t>
         </is>
       </c>
-      <c r="B1076" t="inlineStr"/>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1076" t="inlineStr"/>
     </row>
     <row r="1077">
@@ -13167,7 +13679,11 @@
           <t>Đất Đỏ,BRVT</t>
         </is>
       </c>
-      <c r="B1085" t="inlineStr"/>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1085" t="inlineStr"/>
     </row>
     <row r="1086">
@@ -13215,7 +13731,11 @@
           <t>TP HCM</t>
         </is>
       </c>
-      <c r="B1089" t="inlineStr"/>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1089" t="inlineStr"/>
     </row>
     <row r="1090">
@@ -13263,7 +13783,11 @@
           <t>Huyện Đất Đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1093" t="inlineStr"/>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1093" t="inlineStr"/>
     </row>
     <row r="1094">
@@ -13272,7 +13796,11 @@
           <t>Xuyên Mộc - BRVT</t>
         </is>
       </c>
-      <c r="B1094" t="inlineStr"/>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1094" t="inlineStr"/>
     </row>
     <row r="1095">
@@ -13281,7 +13809,11 @@
           <t>huyện Đất Đỏ tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1095" t="inlineStr"/>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1095" t="inlineStr"/>
     </row>
     <row r="1096">
@@ -13299,7 +13831,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B1097" t="inlineStr"/>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1097" t="inlineStr"/>
     </row>
     <row r="1098">
@@ -13631,7 +14167,11 @@
           <t>Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B1125" t="inlineStr"/>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1125" t="inlineStr"/>
     </row>
     <row r="1126">
@@ -13653,7 +14193,11 @@
           <t>Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1127" t="inlineStr"/>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1127" t="inlineStr"/>
     </row>
     <row r="1128">
@@ -13745,7 +14289,11 @@
           <t>Huyện Đất Đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1135" t="inlineStr"/>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1135" t="inlineStr"/>
     </row>
     <row r="1136">
@@ -13911,7 +14459,11 @@
           <t>Huyện Xuyên Mộc-Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1149" t="inlineStr"/>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1149" t="inlineStr"/>
     </row>
     <row r="1150">
@@ -14021,7 +14573,11 @@
           <t>Huyện đất đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1159" t="inlineStr"/>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1159" t="inlineStr"/>
     </row>
     <row r="1160">
@@ -14092,7 +14648,11 @@
           <t>tân thành, brvt</t>
         </is>
       </c>
-      <c r="B1166" t="inlineStr"/>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1166" t="inlineStr"/>
     </row>
     <row r="1167">
@@ -14179,7 +14739,11 @@
           <t>Đất đỏ, BRVT</t>
         </is>
       </c>
-      <c r="B1173" t="inlineStr"/>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1173" t="inlineStr"/>
     </row>
     <row r="1174">
@@ -14210,7 +14774,11 @@
           <t>Long Điền, brvt</t>
         </is>
       </c>
-      <c r="B1176" t="inlineStr"/>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1176" t="inlineStr"/>
     </row>
     <row r="1177">
@@ -14284,7 +14852,11 @@
           <t>Huyện XM-BRVT</t>
         </is>
       </c>
-      <c r="B1182" t="inlineStr"/>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1182" t="inlineStr"/>
     </row>
     <row r="1183">
@@ -14677,7 +15249,11 @@
           <t>Huyện Đất Đỏ, BRVT</t>
         </is>
       </c>
-      <c r="B1215" t="inlineStr"/>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1215" t="inlineStr"/>
     </row>
     <row r="1216">
@@ -14861,7 +15437,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B1231" t="inlineStr"/>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1231" t="inlineStr"/>
     </row>
     <row r="1232">
@@ -14993,7 +15573,11 @@
           <t>Huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1243" t="inlineStr"/>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1243" t="inlineStr"/>
     </row>
     <row r="1244">
@@ -15050,7 +15634,11 @@
           <t>Xuyen moc brvt</t>
         </is>
       </c>
-      <c r="B1248" t="inlineStr"/>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1248" t="inlineStr"/>
     </row>
     <row r="1249">
@@ -15268,7 +15856,11 @@
           <t>Huyện Đất Đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1266" t="inlineStr"/>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1266" t="inlineStr"/>
     </row>
     <row r="1267">
@@ -15686,7 +16278,11 @@
           <t>Đất Đỏ, BRVT</t>
         </is>
       </c>
-      <c r="B1300" t="inlineStr"/>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1300" t="inlineStr"/>
     </row>
     <row r="1301">
@@ -15836,7 +16432,11 @@
           <t>Đất Đỏ-BRVT</t>
         </is>
       </c>
-      <c r="B1314" t="inlineStr"/>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1314" t="inlineStr"/>
     </row>
     <row r="1315">
@@ -15941,7 +16541,11 @@
           <t>Huyện Đất Đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1323" t="inlineStr"/>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1323" t="inlineStr"/>
     </row>
     <row r="1324">
@@ -15950,7 +16554,11 @@
           <t>Dat Do. Tinh BRVT</t>
         </is>
       </c>
-      <c r="B1324" t="inlineStr"/>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1324" t="inlineStr"/>
     </row>
     <row r="1325">
@@ -15972,7 +16580,11 @@
           <t>Huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1326" t="inlineStr"/>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1326" t="inlineStr"/>
     </row>
     <row r="1327">
@@ -15994,7 +16606,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B1328" t="inlineStr"/>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1328" t="inlineStr"/>
     </row>
     <row r="1329">
@@ -16038,7 +16654,11 @@
           <t>Huyện Đất Đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1332" t="inlineStr"/>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1332" t="inlineStr"/>
     </row>
     <row r="1333">
@@ -16594,7 +17214,11 @@
           <t>Huyện Xuyên Mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1380" t="inlineStr"/>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1380" t="inlineStr"/>
     </row>
     <row r="1381">
@@ -16707,7 +17331,11 @@
           <t>Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1389" t="inlineStr"/>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1389" t="inlineStr"/>
     </row>
     <row r="1390">
@@ -16755,7 +17383,11 @@
           <t>Huyện Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B1393" t="inlineStr"/>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1393" t="inlineStr"/>
     </row>
     <row r="1394">
@@ -16777,7 +17409,11 @@
           <t>Huyện Đất Đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1395" t="inlineStr"/>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1395" t="inlineStr"/>
     </row>
     <row r="1396">
@@ -16891,7 +17527,11 @@
           <t>Huyện Đất đỏ tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1405" t="inlineStr"/>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1405" t="inlineStr"/>
     </row>
     <row r="1406">
@@ -16939,7 +17579,11 @@
           <t>LONG ĐIỀN - BRVT</t>
         </is>
       </c>
-      <c r="B1409" t="inlineStr"/>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1409" t="inlineStr"/>
     </row>
     <row r="1410">
@@ -17074,7 +17718,11 @@
           <t>Xuyên mộc, brvt</t>
         </is>
       </c>
-      <c r="B1420" t="inlineStr"/>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1420" t="inlineStr"/>
     </row>
     <row r="1421">
@@ -17109,7 +17757,11 @@
           <t>H Đất Đỏ- Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1423" t="inlineStr"/>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1423" t="inlineStr"/>
     </row>
     <row r="1424">
@@ -17515,7 +18167,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B1457" t="inlineStr"/>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1457" t="inlineStr"/>
     </row>
     <row r="1458">
@@ -17533,7 +18189,11 @@
           <t>Đất Đỏ, BRVT</t>
         </is>
       </c>
-      <c r="B1459" t="inlineStr"/>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1459" t="inlineStr"/>
     </row>
     <row r="1460">
@@ -17616,7 +18276,11 @@
           <t>Long Điền, Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1466" t="inlineStr"/>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1466" t="inlineStr"/>
     </row>
     <row r="1467">
@@ -17908,7 +18572,11 @@
           <t>TpHCM</t>
         </is>
       </c>
-      <c r="B1490" t="inlineStr"/>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1490" t="inlineStr"/>
     </row>
     <row r="1491">
@@ -17917,7 +18585,11 @@
           <t>TPHCM</t>
         </is>
       </c>
-      <c r="B1491" t="inlineStr"/>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1491" t="inlineStr"/>
     </row>
     <row r="1492">
@@ -18000,7 +18672,11 @@
           <t>Long Điền BRVT</t>
         </is>
       </c>
-      <c r="B1498" t="inlineStr"/>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1498" t="inlineStr"/>
     </row>
     <row r="1499">
@@ -18035,7 +18711,11 @@
           <t>HCM</t>
         </is>
       </c>
-      <c r="B1501" t="inlineStr"/>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1501" t="inlineStr"/>
     </row>
     <row r="1502">
@@ -18057,7 +18737,11 @@
           <t>Long Điền BRVT</t>
         </is>
       </c>
-      <c r="B1503" t="inlineStr"/>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1503" t="inlineStr"/>
     </row>
     <row r="1504">
@@ -18258,7 +18942,11 @@
           <t>Long Điền-BRVT</t>
         </is>
       </c>
-      <c r="B1520" t="inlineStr"/>
+      <c r="B1520" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1520" t="inlineStr"/>
     </row>
     <row r="1521">
@@ -18276,7 +18964,11 @@
           <t>Brvt</t>
         </is>
       </c>
-      <c r="B1522" t="inlineStr"/>
+      <c r="B1522" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1522" t="inlineStr"/>
     </row>
     <row r="1523">
@@ -18464,7 +19156,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B1538" t="inlineStr"/>
+      <c r="B1538" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1538" t="inlineStr"/>
     </row>
     <row r="1539">
@@ -18473,7 +19169,11 @@
           <t>BRVT</t>
         </is>
       </c>
-      <c r="B1539" t="inlineStr"/>
+      <c r="B1539" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1539" t="inlineStr"/>
     </row>
     <row r="1540">
@@ -18626,7 +19326,11 @@
           <t>Huyện Xuyên Mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1552" t="inlineStr"/>
+      <c r="B1552" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1552" t="inlineStr"/>
     </row>
     <row r="1553">
@@ -18683,7 +19387,11 @@
           <t>Huyện Long Điền, Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1557" t="inlineStr"/>
+      <c r="B1557" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1557" t="inlineStr"/>
     </row>
     <row r="1558">
@@ -18714,7 +19422,11 @@
           <t>Xuyên mộc, brvt</t>
         </is>
       </c>
-      <c r="B1560" t="inlineStr"/>
+      <c r="B1560" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1560" t="inlineStr"/>
     </row>
     <row r="1561">
@@ -19007,7 +19719,11 @@
           <t>Long điền, BRVT</t>
         </is>
       </c>
-      <c r="B1585" t="inlineStr"/>
+      <c r="B1585" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1585" t="inlineStr"/>
     </row>
     <row r="1586">
@@ -19238,7 +19954,11 @@
           <t>Huyện Xuyên Mộc, Tỉnh Brvt</t>
         </is>
       </c>
-      <c r="B1604" t="inlineStr"/>
+      <c r="B1604" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1604" t="inlineStr"/>
     </row>
     <row r="1605">
@@ -19339,7 +20059,11 @@
           <t>Long điền brvt</t>
         </is>
       </c>
-      <c r="B1613" t="inlineStr"/>
+      <c r="B1613" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1613" t="inlineStr"/>
     </row>
     <row r="1614">
@@ -19413,7 +20137,11 @@
           <t>Đất đỏ_brvt</t>
         </is>
       </c>
-      <c r="B1619" t="inlineStr"/>
+      <c r="B1619" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1619" t="inlineStr"/>
     </row>
     <row r="1620">
@@ -19596,7 +20324,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B1634" t="inlineStr"/>
+      <c r="B1634" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1634" t="inlineStr"/>
     </row>
     <row r="1635">
@@ -19988,7 +20720,11 @@
           <t>Đất Đỏ, BRVT</t>
         </is>
       </c>
-      <c r="B1666" t="inlineStr"/>
+      <c r="B1666" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1666" t="inlineStr"/>
     </row>
     <row r="1667">
@@ -19997,7 +20733,11 @@
           <t>Huyện Xuyên Mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1667" t="inlineStr"/>
+      <c r="B1667" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1667" t="inlineStr"/>
     </row>
     <row r="1668">
@@ -20237,7 +20977,11 @@
           <t>Quận Bình Tân, TPHCM</t>
         </is>
       </c>
-      <c r="B1687" t="inlineStr"/>
+      <c r="B1687" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1687" t="inlineStr"/>
     </row>
     <row r="1688">
@@ -20299,7 +21043,11 @@
           <t>huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1693" t="inlineStr"/>
+      <c r="B1693" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1693" t="inlineStr"/>
     </row>
     <row r="1694">
@@ -20452,7 +21200,11 @@
           <t>TP HCM</t>
         </is>
       </c>
-      <c r="B1706" t="inlineStr"/>
+      <c r="B1706" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1706" t="inlineStr"/>
     </row>
     <row r="1707">
@@ -20566,7 +21318,11 @@
           <t>Xuyên Mộc,BRVT</t>
         </is>
       </c>
-      <c r="B1716" t="inlineStr"/>
+      <c r="B1716" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1716" t="inlineStr"/>
     </row>
     <row r="1717">
@@ -20636,7 +21392,11 @@
           <t>Long Điền- BRVT</t>
         </is>
       </c>
-      <c r="B1722" t="inlineStr"/>
+      <c r="B1722" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1722" t="inlineStr"/>
     </row>
     <row r="1723">
@@ -20789,7 +21549,11 @@
           <t>Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B1735" t="inlineStr"/>
+      <c r="B1735" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1735" t="inlineStr"/>
     </row>
     <row r="1736">
@@ -20976,7 +21740,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B1750" t="inlineStr"/>
+      <c r="B1750" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1750" t="inlineStr"/>
     </row>
     <row r="1751">
@@ -21176,7 +21944,11 @@
           <t>Xã Phước Hưng- Huyện Long Điền - Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1766" t="inlineStr"/>
+      <c r="B1766" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1766" t="inlineStr"/>
     </row>
     <row r="1767">
@@ -21294,7 +22066,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B1776" t="inlineStr"/>
+      <c r="B1776" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1776" t="inlineStr"/>
     </row>
     <row r="1777">
@@ -21525,7 +22301,11 @@
           <t>Thị xã Phú Mỹ, BRVT</t>
         </is>
       </c>
-      <c r="B1795" t="inlineStr"/>
+      <c r="B1795" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1795" t="inlineStr"/>
     </row>
     <row r="1796">
@@ -21743,7 +22523,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B1813" t="inlineStr"/>
+      <c r="B1813" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1813" t="inlineStr"/>
     </row>
     <row r="1814">
@@ -21801,7 +22585,11 @@
           <t>Huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1819" t="inlineStr"/>
+      <c r="B1819" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1819" t="inlineStr"/>
     </row>
     <row r="1820">
@@ -21932,7 +22720,11 @@
           <t>CHAU DUC, TINH BRVT</t>
         </is>
       </c>
-      <c r="B1830" t="inlineStr"/>
+      <c r="B1830" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1830" t="inlineStr"/>
     </row>
     <row r="1831">
@@ -22054,7 +22846,11 @@
           <t>Huyện Đất Đỏ - Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1840" t="inlineStr"/>
+      <c r="B1840" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1840" t="inlineStr"/>
     </row>
     <row r="1841">
@@ -22142,7 +22938,11 @@
           <t>Huyện Xuyên Mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1848" t="inlineStr"/>
+      <c r="B1848" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1848" t="inlineStr"/>
     </row>
     <row r="1849">
@@ -22216,7 +23016,11 @@
           <t>Tp HCM</t>
         </is>
       </c>
-      <c r="B1854" t="inlineStr"/>
+      <c r="B1854" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1854" t="inlineStr"/>
     </row>
     <row r="1855">
@@ -22361,7 +23165,11 @@
           <t>Tp hcm</t>
         </is>
       </c>
-      <c r="B1867" t="inlineStr"/>
+      <c r="B1867" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1867" t="inlineStr"/>
     </row>
     <row r="1868">
@@ -22370,7 +23178,11 @@
           <t>TPHCM</t>
         </is>
       </c>
-      <c r="B1868" t="inlineStr"/>
+      <c r="B1868" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1868" t="inlineStr"/>
     </row>
     <row r="1869">
@@ -22527,7 +23339,11 @@
           <t>TPHCM</t>
         </is>
       </c>
-      <c r="B1881" t="inlineStr"/>
+      <c r="B1881" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1881" t="inlineStr"/>
     </row>
     <row r="1882">
@@ -22841,7 +23657,11 @@
           <t>BRVT</t>
         </is>
       </c>
-      <c r="B1907" t="inlineStr"/>
+      <c r="B1907" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1907" t="inlineStr"/>
     </row>
     <row r="1908">
@@ -22881,7 +23701,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B1911" t="inlineStr"/>
+      <c r="B1911" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1911" t="inlineStr"/>
     </row>
     <row r="1912">
@@ -22942,7 +23766,11 @@
           <t>BRVT</t>
         </is>
       </c>
-      <c r="B1916" t="inlineStr"/>
+      <c r="B1916" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1916" t="inlineStr"/>
     </row>
     <row r="1917">
@@ -23081,7 +23909,11 @@
           <t>Đất Đỏ-BRVT</t>
         </is>
       </c>
-      <c r="B1927" t="inlineStr"/>
+      <c r="B1927" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1927" t="inlineStr"/>
     </row>
     <row r="1928">
@@ -23182,7 +24014,11 @@
           <t>Long Điền BRVT</t>
         </is>
       </c>
-      <c r="B1936" t="inlineStr"/>
+      <c r="B1936" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1936" t="inlineStr"/>
     </row>
     <row r="1937">
@@ -23217,7 +24053,11 @@
           <t>Huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1939" t="inlineStr"/>
+      <c r="B1939" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1939" t="inlineStr"/>
     </row>
     <row r="1940">
@@ -23252,7 +24092,11 @@
           <t>Long Diền, BRVT</t>
         </is>
       </c>
-      <c r="B1942" t="inlineStr"/>
+      <c r="B1942" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1942" t="inlineStr"/>
     </row>
     <row r="1943">
@@ -23261,7 +24105,11 @@
           <t>Huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1943" t="inlineStr"/>
+      <c r="B1943" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1943" t="inlineStr"/>
     </row>
     <row r="1944">
@@ -23301,7 +24149,11 @@
           <t>Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B1947" t="inlineStr"/>
+      <c r="B1947" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1947" t="inlineStr"/>
     </row>
     <row r="1948">
@@ -23371,7 +24223,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B1953" t="inlineStr"/>
+      <c r="B1953" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1953" t="inlineStr"/>
     </row>
     <row r="1954">
@@ -23459,7 +24315,11 @@
           <t>Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B1961" t="inlineStr"/>
+      <c r="B1961" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1961" t="inlineStr"/>
     </row>
     <row r="1962">
@@ -23646,7 +24506,11 @@
           <t>Long Hải- Long Điền- BRVT</t>
         </is>
       </c>
-      <c r="B1976" t="inlineStr"/>
+      <c r="B1976" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1976" t="inlineStr"/>
     </row>
     <row r="1977">
@@ -23681,7 +24545,11 @@
           <t>Quận 3, tphcm</t>
         </is>
       </c>
-      <c r="B1979" t="inlineStr"/>
+      <c r="B1979" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1979" t="inlineStr"/>
     </row>
     <row r="1980">
@@ -23690,7 +24558,11 @@
           <t>Huyện Long Điền, Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1980" t="inlineStr"/>
+      <c r="B1980" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1980" t="inlineStr"/>
     </row>
     <row r="1981">
@@ -23882,7 +24754,11 @@
           <t>Huyện Xuyên Mộc , tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B1996" t="inlineStr"/>
+      <c r="B1996" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C1996" t="inlineStr"/>
     </row>
     <row r="1997">
@@ -23939,7 +24815,11 @@
           <t>TX Phú Mỹ- BRVT</t>
         </is>
       </c>
-      <c r="B2001" t="inlineStr"/>
+      <c r="B2001" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2001" t="inlineStr"/>
     </row>
     <row r="2002">
@@ -24044,7 +24924,11 @@
           <t>Long Điền. BRVT</t>
         </is>
       </c>
-      <c r="B2010" t="inlineStr"/>
+      <c r="B2010" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2010" t="inlineStr"/>
     </row>
     <row r="2011">
@@ -24414,7 +25298,11 @@
           <t>Long Điền - BRVT</t>
         </is>
       </c>
-      <c r="B2040" t="inlineStr"/>
+      <c r="B2040" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2040" t="inlineStr"/>
     </row>
     <row r="2041">
@@ -24825,7 +25713,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2075" t="inlineStr"/>
+      <c r="B2075" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2075" t="inlineStr"/>
     </row>
     <row r="2076">
@@ -25048,7 +25940,11 @@
           <t>Huyện Long Điền, brvt</t>
         </is>
       </c>
-      <c r="B2094" t="inlineStr"/>
+      <c r="B2094" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2094" t="inlineStr"/>
     </row>
     <row r="2095">
@@ -25066,7 +25962,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2096" t="inlineStr"/>
+      <c r="B2096" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2096" t="inlineStr"/>
     </row>
     <row r="2097">
@@ -25149,7 +26049,11 @@
           <t>Huyện đât đỏ, tỉnh brvt</t>
         </is>
       </c>
-      <c r="B2103" t="inlineStr"/>
+      <c r="B2103" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2103" t="inlineStr"/>
     </row>
     <row r="2104">
@@ -25219,7 +26123,11 @@
           <t>TPHCM</t>
         </is>
       </c>
-      <c r="B2109" t="inlineStr"/>
+      <c r="B2109" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2109" t="inlineStr"/>
     </row>
     <row r="2110">
@@ -25489,7 +26397,11 @@
           <t>Quận Tân Phú, TP HCM</t>
         </is>
       </c>
-      <c r="B2131" t="inlineStr"/>
+      <c r="B2131" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2131" t="inlineStr"/>
     </row>
     <row r="2132">
@@ -25498,7 +26410,11 @@
           <t>tphcm</t>
         </is>
       </c>
-      <c r="B2132" t="inlineStr"/>
+      <c r="B2132" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2132" t="inlineStr"/>
     </row>
     <row r="2133">
@@ -25516,7 +26432,11 @@
           <t>Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B2134" t="inlineStr"/>
+      <c r="B2134" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2134" t="inlineStr"/>
     </row>
     <row r="2135">
@@ -25560,7 +26480,11 @@
           <t>Huyện Châu Đức, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2138" t="inlineStr"/>
+      <c r="B2138" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2138" t="inlineStr"/>
     </row>
     <row r="2139">
@@ -25887,7 +26811,11 @@
           <t>Huyện Xuyên Mộc, tĩnh BRVT</t>
         </is>
       </c>
-      <c r="B2165" t="inlineStr"/>
+      <c r="B2165" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2165" t="inlineStr"/>
     </row>
     <row r="2166">
@@ -25896,7 +26824,11 @@
           <t>Huyện Xuyên  Mộc - BRVT</t>
         </is>
       </c>
-      <c r="B2166" t="inlineStr"/>
+      <c r="B2166" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2166" t="inlineStr"/>
     </row>
     <row r="2167">
@@ -25992,7 +26924,11 @@
           <t>Cần Giờ, tp.HCM</t>
         </is>
       </c>
-      <c r="B2174" t="inlineStr"/>
+      <c r="B2174" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2174" t="inlineStr"/>
     </row>
     <row r="2175">
@@ -26014,7 +26950,11 @@
           <t>Cần Giờ, TP.HCM</t>
         </is>
       </c>
-      <c r="B2176" t="inlineStr"/>
+      <c r="B2176" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2176" t="inlineStr"/>
     </row>
     <row r="2177">
@@ -26743,7 +27683,11 @@
           <t>Huyện Đất Đỏ-Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2237" t="inlineStr"/>
+      <c r="B2237" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2237" t="inlineStr"/>
     </row>
     <row r="2238">
@@ -26752,7 +27696,11 @@
           <t>Huyện Long Điền -BRVT</t>
         </is>
       </c>
-      <c r="B2238" t="inlineStr"/>
+      <c r="B2238" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2238" t="inlineStr"/>
     </row>
     <row r="2239">
@@ -26809,7 +27757,11 @@
           <t>LONG ĐIỀN- BRVT</t>
         </is>
       </c>
-      <c r="B2243" t="inlineStr"/>
+      <c r="B2243" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2243" t="inlineStr"/>
     </row>
     <row r="2244">
@@ -26914,7 +27866,11 @@
           <t>Xuyên Mộc - BRVT</t>
         </is>
       </c>
-      <c r="B2252" t="inlineStr"/>
+      <c r="B2252" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2252" t="inlineStr"/>
     </row>
     <row r="2253">
@@ -26923,7 +27879,11 @@
           <t>Huyện Xuyên Mộc, Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2253" t="inlineStr"/>
+      <c r="B2253" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2253" t="inlineStr"/>
     </row>
     <row r="2254">
@@ -26976,7 +27936,11 @@
           <t>XMBRVT</t>
         </is>
       </c>
-      <c r="B2258" t="inlineStr"/>
+      <c r="B2258" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2258" t="inlineStr"/>
     </row>
     <row r="2259">
@@ -27059,7 +28023,11 @@
           <t>Huyên Xuyên Mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2265" t="inlineStr"/>
+      <c r="B2265" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2265" t="inlineStr"/>
     </row>
     <row r="2266">
@@ -27208,7 +28176,11 @@
           <t>HCM</t>
         </is>
       </c>
-      <c r="B2278" t="inlineStr"/>
+      <c r="B2278" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2278" t="inlineStr"/>
     </row>
     <row r="2279">
@@ -27217,7 +28189,11 @@
           <t>Xuyên Mộc - BRVT</t>
         </is>
       </c>
-      <c r="B2279" t="inlineStr"/>
+      <c r="B2279" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2279" t="inlineStr"/>
     </row>
     <row r="2280">
@@ -27401,7 +28377,11 @@
           <t>Cần Giờ -to  HCM</t>
         </is>
       </c>
-      <c r="B2295" t="inlineStr"/>
+      <c r="B2295" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2295" t="inlineStr"/>
     </row>
     <row r="2296">
@@ -27541,7 +28521,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2307" t="inlineStr"/>
+      <c r="B2307" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2307" t="inlineStr"/>
     </row>
     <row r="2308">
@@ -27889,7 +28873,11 @@
           <t>H. Xuyên mộc, t. Brvt</t>
         </is>
       </c>
-      <c r="B2335" t="inlineStr"/>
+      <c r="B2335" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2335" t="inlineStr"/>
     </row>
     <row r="2336">
@@ -27933,7 +28921,11 @@
           <t>Huyện Long Điền tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2339" t="inlineStr"/>
+      <c r="B2339" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2339" t="inlineStr"/>
     </row>
     <row r="2340">
@@ -28016,7 +29008,11 @@
           <t>Huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2346" t="inlineStr"/>
+      <c r="B2346" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2346" t="inlineStr"/>
     </row>
     <row r="2347">
@@ -28148,7 +29144,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2358" t="inlineStr"/>
+      <c r="B2358" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2358" t="inlineStr"/>
     </row>
     <row r="2359">
@@ -28166,7 +29166,11 @@
           <t>Châu Đức, BRVT</t>
         </is>
       </c>
-      <c r="B2360" t="inlineStr"/>
+      <c r="B2360" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2360" t="inlineStr"/>
     </row>
     <row r="2361">
@@ -28456,7 +29460,11 @@
           <t>BRVT</t>
         </is>
       </c>
-      <c r="B2386" t="inlineStr"/>
+      <c r="B2386" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2386" t="inlineStr"/>
     </row>
     <row r="2387">
@@ -28764,7 +29772,11 @@
           <t>Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2410" t="inlineStr"/>
+      <c r="B2410" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2410" t="inlineStr"/>
     </row>
     <row r="2411">
@@ -28773,7 +29785,11 @@
           <t>châu đức-brvt</t>
         </is>
       </c>
-      <c r="B2411" t="inlineStr"/>
+      <c r="B2411" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2411" t="inlineStr"/>
     </row>
     <row r="2412">
@@ -28808,7 +29824,11 @@
           <t>Huyện Xuyên Mộc, Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2414" t="inlineStr"/>
+      <c r="B2414" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2414" t="inlineStr"/>
     </row>
     <row r="2415">
@@ -28830,7 +29850,11 @@
           <t>Huyện xuyên mộc tỉnh brvt</t>
         </is>
       </c>
-      <c r="B2416" t="inlineStr"/>
+      <c r="B2416" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2416" t="inlineStr"/>
     </row>
     <row r="2417">
@@ -28865,7 +29889,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2419" t="inlineStr"/>
+      <c r="B2419" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2419" t="inlineStr"/>
     </row>
     <row r="2420">
@@ -28900,7 +29928,11 @@
           <t>XUYÊN MỘC- BRVT</t>
         </is>
       </c>
-      <c r="B2422" t="inlineStr"/>
+      <c r="B2422" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2422" t="inlineStr"/>
     </row>
     <row r="2423">
@@ -28935,7 +29967,11 @@
           <t>Xuyên Mộc,BRVT</t>
         </is>
       </c>
-      <c r="B2425" t="inlineStr"/>
+      <c r="B2425" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2425" t="inlineStr"/>
     </row>
     <row r="2426">
@@ -28944,7 +29980,11 @@
           <t>Xuyên Mộc - BRVT</t>
         </is>
       </c>
-      <c r="B2426" t="inlineStr"/>
+      <c r="B2426" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2426" t="inlineStr"/>
     </row>
     <row r="2427">
@@ -28975,7 +30015,11 @@
           <t>Long Điền, BRVT</t>
         </is>
       </c>
-      <c r="B2429" t="inlineStr"/>
+      <c r="B2429" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2429" t="inlineStr"/>
     </row>
     <row r="2430">
@@ -29081,7 +30125,11 @@
           <t>Huyện xuyên Mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2439" t="inlineStr"/>
+      <c r="B2439" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2439" t="inlineStr"/>
     </row>
     <row r="2440">
@@ -29099,7 +30147,11 @@
           <t>Huyện Xuyên Mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2441" t="inlineStr"/>
+      <c r="B2441" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2441" t="inlineStr"/>
     </row>
     <row r="2442">
@@ -29130,7 +30182,11 @@
           <t>Huyện Xuyên Mộc , tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2444" t="inlineStr"/>
+      <c r="B2444" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2444" t="inlineStr"/>
     </row>
     <row r="2445">
@@ -29139,7 +30195,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2445" t="inlineStr"/>
+      <c r="B2445" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2445" t="inlineStr"/>
     </row>
     <row r="2446">
@@ -29170,7 +30230,11 @@
           <t>Huyện Xuyên Mộc, Tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2448" t="inlineStr"/>
+      <c r="B2448" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2448" t="inlineStr"/>
     </row>
     <row r="2449">
@@ -29280,7 +30344,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2458" t="inlineStr"/>
+      <c r="B2458" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2458" t="inlineStr"/>
     </row>
     <row r="2459">
@@ -29328,7 +30396,11 @@
           <t>Xuyên Mộc , BRVT</t>
         </is>
       </c>
-      <c r="B2462" t="inlineStr"/>
+      <c r="B2462" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2462" t="inlineStr"/>
     </row>
     <row r="2463">
@@ -29433,7 +30505,11 @@
           <t>Huyện Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2471" t="inlineStr"/>
+      <c r="B2471" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2471" t="inlineStr"/>
     </row>
     <row r="2472">
@@ -29477,7 +30553,11 @@
           <t>Xuyên Mộc BRVT</t>
         </is>
       </c>
-      <c r="B2475" t="inlineStr"/>
+      <c r="B2475" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2475" t="inlineStr"/>
     </row>
     <row r="2476">
@@ -29525,7 +30605,11 @@
           <t>Xuyên mộc, brvt</t>
         </is>
       </c>
-      <c r="B2479" t="inlineStr"/>
+      <c r="B2479" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2479" t="inlineStr"/>
     </row>
     <row r="2480">
@@ -29582,7 +30666,11 @@
           <t>Xuyên mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2484" t="inlineStr"/>
+      <c r="B2484" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2484" t="inlineStr"/>
     </row>
     <row r="2485">
@@ -29739,7 +30827,11 @@
           <t>Xuyên Mộc BRVT</t>
         </is>
       </c>
-      <c r="B2497" t="inlineStr"/>
+      <c r="B2497" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2497" t="inlineStr"/>
     </row>
     <row r="2498">
@@ -29800,7 +30892,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2502" t="inlineStr"/>
+      <c r="B2502" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2502" t="inlineStr"/>
     </row>
     <row r="2503">
@@ -30488,7 +31584,11 @@
           <t>TPHCM</t>
         </is>
       </c>
-      <c r="B2558" t="inlineStr"/>
+      <c r="B2558" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2558" t="inlineStr"/>
     </row>
     <row r="2559">
@@ -30767,7 +31867,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2581" t="inlineStr"/>
+      <c r="B2581" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2581" t="inlineStr"/>
     </row>
     <row r="2582">
@@ -30824,7 +31928,11 @@
           <t>Huyện xuyên mộc - brvt</t>
         </is>
       </c>
-      <c r="B2586" t="inlineStr"/>
+      <c r="B2586" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2586" t="inlineStr"/>
     </row>
     <row r="2587">
@@ -30833,7 +31941,11 @@
           <t>Phú mỹ,BRVT</t>
         </is>
       </c>
-      <c r="B2587" t="inlineStr"/>
+      <c r="B2587" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2587" t="inlineStr"/>
     </row>
     <row r="2588">
@@ -30855,7 +31967,11 @@
           <t>Tphcm</t>
         </is>
       </c>
-      <c r="B2589" t="inlineStr"/>
+      <c r="B2589" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2589" t="inlineStr"/>
     </row>
     <row r="2590">
@@ -31273,7 +32389,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2623" t="inlineStr"/>
+      <c r="B2623" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2623" t="inlineStr"/>
     </row>
     <row r="2624">
@@ -31291,7 +32411,11 @@
           <t>Đất Đỏ- BRVT</t>
         </is>
       </c>
-      <c r="B2625" t="inlineStr"/>
+      <c r="B2625" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2625" t="inlineStr"/>
     </row>
     <row r="2626">
@@ -31309,7 +32433,11 @@
           <t>Huyện Châu Đức, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2627" t="inlineStr"/>
+      <c r="B2627" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2627" t="inlineStr"/>
     </row>
     <row r="2628">
@@ -31384,7 +32512,11 @@
           <t>Huyện Long Điền, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2634" t="inlineStr"/>
+      <c r="B2634" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2634" t="inlineStr"/>
     </row>
     <row r="2635">
@@ -31520,7 +32652,11 @@
           <t>BRVT</t>
         </is>
       </c>
-      <c r="B2646" t="inlineStr"/>
+      <c r="B2646" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2646" t="inlineStr"/>
     </row>
     <row r="2647">
@@ -31625,7 +32761,11 @@
           <t>Bình Thạnh, HCM</t>
         </is>
       </c>
-      <c r="B2655" t="inlineStr"/>
+      <c r="B2655" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2655" t="inlineStr"/>
     </row>
     <row r="2656">
@@ -31634,7 +32774,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2656" t="inlineStr"/>
+      <c r="B2656" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2656" t="inlineStr"/>
     </row>
     <row r="2657">
@@ -31854,7 +32998,11 @@
           <t>Huyện Đất Đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2676" t="inlineStr"/>
+      <c r="B2676" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2676" t="inlineStr"/>
     </row>
     <row r="2677">
@@ -31863,7 +33011,11 @@
           <t>Huyện Đất Đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2677" t="inlineStr"/>
+      <c r="B2677" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2677" t="inlineStr"/>
     </row>
     <row r="2678">
@@ -31872,7 +33024,11 @@
           <t>Thị Xã Phú Mỹ BRVT</t>
         </is>
       </c>
-      <c r="B2678" t="inlineStr"/>
+      <c r="B2678" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2678" t="inlineStr"/>
     </row>
     <row r="2679">
@@ -31960,7 +33116,11 @@
           <t>BRVT</t>
         </is>
       </c>
-      <c r="B2686" t="inlineStr"/>
+      <c r="B2686" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2686" t="inlineStr"/>
     </row>
     <row r="2687">
@@ -32039,7 +33199,11 @@
           <t>Quận 6- TpHCM</t>
         </is>
       </c>
-      <c r="B2693" t="inlineStr"/>
+      <c r="B2693" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2693" t="inlineStr"/>
     </row>
     <row r="2694">
@@ -32092,7 +33256,11 @@
           <t>Xuyên Mộc, Brvt</t>
         </is>
       </c>
-      <c r="B2698" t="inlineStr"/>
+      <c r="B2698" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2698" t="inlineStr"/>
     </row>
     <row r="2699">
@@ -32136,7 +33304,11 @@
           <t>TP HCM</t>
         </is>
       </c>
-      <c r="B2702" t="inlineStr"/>
+      <c r="B2702" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2702" t="inlineStr"/>
     </row>
     <row r="2703">
@@ -32280,7 +33452,11 @@
           <t>Huyện long điền tỉnh brvt</t>
         </is>
       </c>
-      <c r="B2714" t="inlineStr"/>
+      <c r="B2714" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2714" t="inlineStr"/>
     </row>
     <row r="2715">
@@ -32289,7 +33465,11 @@
           <t>Huyện Long điền tỉnh brvt</t>
         </is>
       </c>
-      <c r="B2715" t="inlineStr"/>
+      <c r="B2715" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2715" t="inlineStr"/>
     </row>
     <row r="2716">
@@ -32369,7 +33549,11 @@
           <t>Xuyên Mộc, Brvt</t>
         </is>
       </c>
-      <c r="B2723" t="inlineStr"/>
+      <c r="B2723" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2723" t="inlineStr"/>
     </row>
     <row r="2724">
@@ -32435,7 +33619,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2729" t="inlineStr"/>
+      <c r="B2729" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2729" t="inlineStr"/>
     </row>
     <row r="2730">
@@ -32444,7 +33632,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2730" t="inlineStr"/>
+      <c r="B2730" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2730" t="inlineStr"/>
     </row>
     <row r="2731">
@@ -32497,7 +33689,11 @@
           <t>Huyện Đất Đỏ, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2735" t="inlineStr"/>
+      <c r="B2735" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2735" t="inlineStr"/>
     </row>
     <row r="2736">
@@ -32937,7 +34133,11 @@
           <t>Huyện đất đỏ - BRVT</t>
         </is>
       </c>
-      <c r="B2771" t="inlineStr"/>
+      <c r="B2771" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2771" t="inlineStr"/>
     </row>
     <row r="2772">
@@ -32968,7 +34168,11 @@
           <t>Xuyên mộc, brvt</t>
         </is>
       </c>
-      <c r="B2774" t="inlineStr"/>
+      <c r="B2774" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2774" t="inlineStr"/>
     </row>
     <row r="2775">
@@ -33138,7 +34342,11 @@
           <t>Huyện Xuyên Mộc BRVT</t>
         </is>
       </c>
-      <c r="B2788" t="inlineStr"/>
+      <c r="B2788" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2788" t="inlineStr"/>
     </row>
     <row r="2789">
@@ -33147,7 +34355,11 @@
           <t>Xuyên mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2789" t="inlineStr"/>
+      <c r="B2789" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2789" t="inlineStr"/>
     </row>
     <row r="2790">
@@ -33156,7 +34368,11 @@
           <t>Xuyên Mộc,BRVT</t>
         </is>
       </c>
-      <c r="B2790" t="inlineStr"/>
+      <c r="B2790" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2790" t="inlineStr"/>
     </row>
     <row r="2791">
@@ -33165,7 +34381,11 @@
           <t>Xuyên Mộc, BRVT</t>
         </is>
       </c>
-      <c r="B2791" t="inlineStr"/>
+      <c r="B2791" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2791" t="inlineStr"/>
     </row>
     <row r="2792">
@@ -33183,7 +34403,11 @@
           <t>xuyen moc, brvt</t>
         </is>
       </c>
-      <c r="B2793" t="inlineStr"/>
+      <c r="B2793" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2793" t="inlineStr"/>
     </row>
     <row r="2794">
@@ -33201,7 +34425,11 @@
           <t>Xuyên mộc brvt</t>
         </is>
       </c>
-      <c r="B2795" t="inlineStr"/>
+      <c r="B2795" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2795" t="inlineStr"/>
     </row>
     <row r="2796">
@@ -33254,7 +34482,11 @@
           <t>Xuyên Mộc . BRVT</t>
         </is>
       </c>
-      <c r="B2800" t="inlineStr"/>
+      <c r="B2800" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2800" t="inlineStr"/>
     </row>
     <row r="2801">
@@ -33554,7 +34786,11 @@
           <t>Huyện Xuyên Mộc, tỉnh BRVT</t>
         </is>
       </c>
-      <c r="B2824" t="inlineStr"/>
+      <c r="B2824" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2824" t="inlineStr"/>
     </row>
     <row r="2825">
@@ -33778,7 +35014,11 @@
           <t>Huyện Hóc Môn, TP. HCM</t>
         </is>
       </c>
-      <c r="B2844" t="inlineStr"/>
+      <c r="B2844" t="inlineStr">
+        <is>
+          <t>Đông Nam Bộ</t>
+        </is>
+      </c>
       <c r="C2844" t="inlineStr"/>
     </row>
     <row r="2845">

</xml_diff>

<commit_message>
add new func find area from TayBac.txt
</commit_message>
<xml_diff>
--- a/updated_Vung-Khuvuc.xlsx
+++ b/updated_Vung-Khuvuc.xlsx
@@ -461,7 +461,11 @@
           <t>Tây Bắc Bộ</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Nông Thôn</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -25081,7 +25085,11 @@
           <t>Tây Bắc Bộ</t>
         </is>
       </c>
-      <c r="C2022" t="inlineStr"/>
+      <c r="C2022" t="inlineStr">
+        <is>
+          <t>Nông Thôn</t>
+        </is>
+      </c>
     </row>
     <row r="2023">
       <c r="A2023" t="inlineStr">

</xml_diff>